<commit_message>
small changes in model and components about delay distributions and break probabilities
</commit_message>
<xml_diff>
--- a/data/natural_hazards.xlsx
+++ b/data/natural_hazards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyasl\PycharmProjects\AS-Lab4\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBF78C4-DC81-4BDB-BDB9-39A792A5BA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F874DA18-B520-4ABD-B081-46530241D2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{C36D3B4C-DD6F-40D3-B74A-A792DAE97B6C}"/>
   </bookViews>
@@ -18,6 +18,10 @@
     <sheet name="Cyclone" sheetId="4" r:id="rId3"/>
     <sheet name="Flood" sheetId="3" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Earthquake!$A$1:$C$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Erosion!$A$1:$C$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="87">
   <si>
     <t>Bagerhat</t>
   </si>
@@ -259,9 +263,6 @@
     <t>Bogura</t>
   </si>
   <si>
-    <t>Narshingdi</t>
-  </si>
-  <si>
     <t>Panchagarh</t>
   </si>
   <si>
@@ -274,15 +275,9 @@
     <t>Gaibandha</t>
   </si>
   <si>
-    <t>Hobiganj</t>
-  </si>
-  <si>
     <t>Keshoreganj</t>
   </si>
   <si>
-    <t>Moulvibazar</t>
-  </si>
-  <si>
     <t>Division</t>
   </si>
   <si>
@@ -295,12 +290,6 @@
     <t>Almost Certain</t>
   </si>
   <si>
-    <t xml:space="preserve">Shariatpur </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tangail </t>
-  </si>
-  <si>
     <t xml:space="preserve">Satkhira </t>
   </si>
   <si>
@@ -311,6 +300,9 @@
   </si>
   <si>
     <t>Vulnerability score</t>
+  </si>
+  <si>
+    <t>Laxmipur</t>
   </si>
 </sst>
 </file>
@@ -366,10 +358,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -671,24 +659,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A3DCEC-55FC-4F07-B5AA-2F3566B54D9B}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -704,18 +693,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C3">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>64</v>
@@ -726,7 +715,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>64</v>
@@ -737,7 +726,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>64</v>
@@ -748,51 +737,51 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C7">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C9">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C10">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -803,51 +792,51 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C13">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C15">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>64</v>
@@ -858,40 +847,40 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C17">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C18">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>64</v>
@@ -902,29 +891,29 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C21">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C22">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
@@ -935,7 +924,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
@@ -946,18 +935,18 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>66</v>
@@ -968,18 +957,18 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C27">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
         <v>66</v>
@@ -990,84 +979,84 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C29">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C30">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>73</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C33">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
         <v>66</v>
@@ -1078,29 +1067,29 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C38">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>66</v>
@@ -1111,18 +1100,18 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C40">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
         <v>66</v>
@@ -1133,18 +1122,18 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C42">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>8</v>
+      <c r="A43" t="s">
+        <v>40</v>
       </c>
       <c r="B43" t="s">
         <v>66</v>
@@ -1155,7 +1144,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>66</v>
@@ -1166,7 +1155,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
         <v>66</v>
@@ -1177,7 +1166,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
         <v>66</v>
@@ -1188,18 +1177,18 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C47">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
         <v>66</v>
@@ -1210,18 +1199,18 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C49">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
         <v>66</v>
@@ -1232,7 +1221,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
         <v>66</v>
@@ -1243,62 +1232,62 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C52">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C53">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C54">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C55">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C56">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
         <v>67</v>
@@ -1309,29 +1298,29 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C58">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C59">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
         <v>67</v>
@@ -1342,18 +1331,18 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C61">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
         <v>67</v>
@@ -1375,135 +1364,143 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C64">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C65" xr:uid="{84A3DCEC-55FC-4F07-B5AA-2F3566B54D9B}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C65">
+      <sortCondition ref="A1:A65"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A9FFB1-1552-44AB-B4B6-9753BB14DB58}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>8</v>
+      <c r="A4" t="s">
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>46</v>
+      <c r="A7" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>53</v>
+      <c r="A9" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1511,21 +1508,21 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1533,62 +1530,62 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C12">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="C13">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>34</v>
+      <c r="A15" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C15">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C16">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>39</v>
+      <c r="A17" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
@@ -1598,8 +1595,8 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>44</v>
+      <c r="A18" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
@@ -1609,41 +1606,41 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>57</v>
+      <c r="A19" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C19">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C20">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21">
         <v>0</v>
-      </c>
-      <c r="B21" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21">
-        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
         <v>66</v>
@@ -1654,40 +1651,40 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C23">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>26</v>
+      <c r="A24" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>67</v>
@@ -1698,51 +1695,51 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C27">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>71</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C28">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>31</v>
+      <c r="A29" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C29">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C30">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
         <v>67</v>
@@ -1753,43 +1750,43 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>3</v>
+      <c r="A34" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1797,10 +1794,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1808,10 +1805,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1819,10 +1816,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1830,54 +1827,54 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="C40">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>30</v>
+      <c r="A41" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1885,32 +1882,32 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>58</v>
+      <c r="A46" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1918,16 +1915,32 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48">
+        <v>0.25</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C47" xr:uid="{38A9FFB1-1552-44AB-B4B6-9753BB14DB58}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C47">
+      <sortCondition ref="A1:A47"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1937,7 +1950,7 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,13 +1960,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2717,13 +2730,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2731,7 +2744,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2742,7 +2755,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2753,7 +2766,7 @@
         <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -2764,7 +2777,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2775,7 +2788,7 @@
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -2783,10 +2796,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -2827,7 +2840,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -2904,7 +2917,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>64</v>
@@ -3003,7 +3016,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
         <v>64</v>
@@ -3135,7 +3148,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
@@ -3182,7 +3195,7 @@
         <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3193,7 +3206,7 @@
         <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -3204,7 +3217,7 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -3215,7 +3228,7 @@
         <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3223,10 +3236,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C47">
         <v>1</v>
@@ -3237,7 +3250,7 @@
         <v>20</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -3248,7 +3261,7 @@
         <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -3259,7 +3272,7 @@
         <v>30</v>
       </c>
       <c r="B50" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3270,7 +3283,7 @@
         <v>36</v>
       </c>
       <c r="B51" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3281,7 +3294,7 @@
         <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -3292,7 +3305,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C53">
         <v>1</v>
@@ -3303,7 +3316,7 @@
         <v>40</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -3314,7 +3327,7 @@
         <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3325,7 +3338,7 @@
         <v>51</v>
       </c>
       <c r="B56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -3336,7 +3349,7 @@
         <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3347,7 +3360,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3358,7 +3371,7 @@
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3369,7 +3382,7 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C60">
         <v>1</v>

</xml_diff>

<commit_message>
Scenario CSVs are ready!
</commit_message>
<xml_diff>
--- a/data/natural_hazards.xlsx
+++ b/data/natural_hazards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyasl\PycharmProjects\AS-Lab4\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F874DA18-B520-4ABD-B081-46530241D2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67833D0A-DF59-4578-9E69-91084FB4AFF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{C36D3B4C-DD6F-40D3-B74A-A792DAE97B6C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{C36D3B4C-DD6F-40D3-B74A-A792DAE97B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Earthquake" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Earthquake!$A$1:$C$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Erosion!$A$1:$C$47</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Flood!$A$1:$C$60</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="84">
   <si>
     <t>Bagerhat</t>
   </si>
@@ -260,16 +261,7 @@
     <t>Lakshmipur</t>
   </si>
   <si>
-    <t>Bogura</t>
-  </si>
-  <si>
     <t>Panchagarh</t>
-  </si>
-  <si>
-    <t>Cumilla</t>
-  </si>
-  <si>
-    <t>Cox’s Bazar</t>
   </si>
   <si>
     <t>Gaibandha</t>
@@ -671,13 +663,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1012,7 +1004,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
         <v>64</v>
@@ -1409,13 +1401,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1434,7 +1426,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1445,7 +1437,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1456,7 +1448,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1467,7 +1459,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1478,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1489,7 +1481,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1500,7 +1492,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1522,7 +1514,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1544,7 +1536,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1555,7 +1547,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1566,7 +1558,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1610,7 +1602,7 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1632,7 +1624,7 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1654,7 +1646,7 @@
         <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -1662,7 +1654,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
         <v>67</v>
@@ -1676,7 +1668,7 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1764,7 +1756,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1775,7 +1767,7 @@
         <v>48</v>
       </c>
       <c r="B34" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1786,7 +1778,7 @@
         <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C35">
         <v>1</v>
@@ -1797,7 +1789,7 @@
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -1808,7 +1800,7 @@
         <v>51</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C37">
         <v>1</v>
@@ -1819,7 +1811,7 @@
         <v>51</v>
       </c>
       <c r="B38" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -1830,7 +1822,7 @@
         <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -1874,7 +1866,7 @@
         <v>58</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -1885,7 +1877,7 @@
         <v>59</v>
       </c>
       <c r="B44" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1907,7 +1899,7 @@
         <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -1918,7 +1910,7 @@
         <v>62</v>
       </c>
       <c r="B47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -1949,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C2661B3-1B20-40B6-90F9-0FC19F04AA94}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,13 +1952,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2720,31 +2712,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DC4B93-9F3A-48EC-9DB3-5A7985586090}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -2752,10 +2747,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -2763,68 +2758,68 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C9">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2840,7 +2835,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>64</v>
@@ -2851,7 +2846,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
@@ -2862,29 +2857,29 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C13">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C14">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>64</v>
@@ -2895,18 +2890,18 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C16">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
@@ -2917,51 +2912,51 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C18">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C19">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C20">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C21">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
         <v>64</v>
@@ -2972,7 +2967,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>64</v>
@@ -2983,7 +2978,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
@@ -2994,7 +2989,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="B25" t="s">
         <v>64</v>
@@ -3005,51 +3000,51 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C26">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C27">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C28">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C29">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="B30" t="s">
         <v>66</v>
@@ -3060,18 +3055,18 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C31">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>66</v>
@@ -3082,51 +3077,51 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C34">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="C36">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>66</v>
@@ -3137,35 +3132,35 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C38">
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C39">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3181,54 +3176,54 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C42">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -3236,43 +3231,43 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C47">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C49">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -3280,10 +3275,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -3291,43 +3286,43 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C53">
-        <v>1</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="B54" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C55">
         <v>1</v>
@@ -3335,21 +3330,21 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C56">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3357,21 +3352,21 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3379,16 +3374,54 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B60" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C60">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C62">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C60" xr:uid="{C6DC4B93-9F3A-48EC-9DB3-5A7985586090}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C60">
+      <sortCondition ref="A1:A60"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>